<commit_message>
added 3 new scripts and input excels
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Bento_MultiFilter_Diagnosis-Recurrence-TumorSize-Chemo_1.xlsx
+++ b/InputFiles/TC01_Bento_MultiFilter_Diagnosis-Recurrence-TumorSize-Chemo_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A2F27D-4C20-4466-BD32-927262997EBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CBC0FFA-DF0B-4EAE-B6A1-84157EF8DC35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="60" yWindow="10" windowWidth="19140" windowHeight="10190" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -522,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
updated the filters for perf script
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Bento_MultiFilter_Diagnosis-Recurrence-TumorSize-Chemo_1.xlsx
+++ b/InputFiles/TC01_Bento_MultiFilter_Diagnosis-Recurrence-TumorSize-Chemo_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CBC0FFA-DF0B-4EAE-B6A1-84157EF8DC35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3D89D3-8382-4D9A-A92F-6EF760CD3BC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="10" windowWidth="19140" windowHeight="10190" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -64,25 +64,43 @@
   </si>
   <si>
     <t>MATCH (ss:study_subject)
-MATCH (ss)&lt;-[:sample_of_study_subject]-(sp)&lt;-[:file_of_sample]-(f)-[:file_of_laboratory_procedure]-&gt;(lp)
-WITH ss, collect(DISTINCT sp.sample_id) AS samples, collect(DISTINCT lp.laboratory_procedure_id) AS lab_procedures, collect(DISTINCT f) AS files
-MATCH (ss)-[:study_subject_of_study]-&gt;(s)-[:study_of_program]-&gt;(p)
 MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
 MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
 MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
-MATCH (ss)&lt;-[:demographic_of_study_subject]-(demo)
- WHERE ss.disease_subtype IN ["Medullary Carcinoma"] and sf.grouped_recurrence_score IN ["16-20"]and d.tumor_size_group In ["(2,3]"] and tp.chemotherapy_regimen In ["FEC (3 week cycles)"]
-return ss.study_subject_id as `Case ID`,
-       p.program_acronym as `Program Code`,
-        p.program_id as Program_ID,
-       s.study_acronym as `Arm`,
-       ss.disease_subtype as `Diagnosis`,
-       sf.grouped_recurrence_score AS `Recurrence Score`,
-       d.tumor_size_group AS `tumor_size`,
-       d.er_status AS `ER Status`,
-       d.pr_status AS `PR Status`,
-       demo.age_at_index AS `Age (years)`,
-demo.survival_time AS `Survival (days)`</t>
+WHERE ss.disease_subtype IN ["Medullary Carcinoma"] and sf.grouped_recurrence_score IN ["16-20"]and d.tumor_size_group In ["(2,3]"] and tp.chemotherapy_regimen In ["Other treatment given as part of a CTSU protocol"]
+WITH ss
+MATCH (ss)-[:study_subject_of_study]-&gt;(s)
+MATCH (s)-[:study_of_program]-&gt;(p)
+MATCH (ss)&lt;-[:sample_of_study_subject]-(samp)
+MATCH (samp)&lt;-[:file_of_sample]-(f)
+MATCH (lp)&lt;-[:file_of_laboratory_procedure]-(f)
+RETURN COUNT(DISTINCT p) AS Programs,
+COUNT(DISTINCT s) AS Arms,
+COUNT(DISTINCT ss) AS Cases,
+COUNT(DISTINCT samp) AS Samples,
+COUNT(DISTINCT lp) AS Assays,
+COUNT(DISTINCT f) AS Files</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)
+MATCH (f)-[:file_of_sample]-&gt;(samp)
+MATCH (samp)-[:sample_of_study_subject]-&gt;(ss)
+MATCH (ss)-[:study_subject_of_study]-&gt;(s)
+MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
+MATCH (s)-[:study_of_program]-&gt;(p)
+MATCH (d)-[:diagnosis_of_study_subject]-&gt;(ss)
+MATCH (tp)-[:tp_of_diagnosis]-&gt;(d)
+WHERE ss.disease_subtype IN ["Medullary Carcinoma"] and sf.grouped_recurrence_score IN ["16-20"]and d.tumor_size_group In ["(2,3]"] and tp.chemotherapy_regimen In ["Other treatment given as part of a CTSU protocol"]
+RETURN  f.file_name AS `File Name`,
+    head(labels(samp)) AS `Association`,
+    f.file_description AS `Description`,
+    f.file_format AS `File Format`,
+    f.file_size AS `Size`,
+    p.program_acronym AS `Program Code`,
+    s.study_acronym AS `Arm`,
+    ss.study_subject_id AS `Case ID`,
+    samp.sample_id AS `Sample ID`,
+    ss.disease_subtype as `Diagnosis`</t>
   </si>
   <si>
     <t>MATCH (ss:study_subject)
@@ -94,7 +112,7 @@
 MATCH (samp)&lt;-[:file_of_sample]-(f)-[:file_of_laboratory_procedure]-&gt;(lp)
 MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
 MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
-WHERE ss.disease_subtype IN ["Medullary Carcinoma"] and sf.grouped_recurrence_score IN ["16-20"]and d.tumor_size_group In ["(2,3]"] and tp.chemotherapy_regimen In ["FEC (3 week cycles)"]
+WHERE ss.disease_subtype IN ["Medullary Carcinoma"] and sf.grouped_recurrence_score IN ["16-20"]and d.tumor_size_group In ["(2,3]"] and tp.chemotherapy_regimen In ["Other treatment given as part of a CTSU protocol"]
 WITH
     distinct lp,
     toInteger(split(ss.study_subject_id,'-')[2]) AS subject_id_num,
@@ -113,44 +131,26 @@
             lp.test_name as Platform</t>
   </si>
   <si>
-    <t>MATCH (f:file)
-MATCH (f)-[:file_of_sample]-&gt;(samp)
-MATCH (samp)-[:sample_of_study_subject]-&gt;(ss)
-MATCH (ss)-[:study_subject_of_study]-&gt;(s)
-MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
-MATCH (s)-[:study_of_program]-&gt;(p)
-MATCH (d)-[:diagnosis_of_study_subject]-&gt;(ss)
-MATCH (tp)-[:tp_of_diagnosis]-&gt;(d)
-WHERE ss.disease_subtype IN ["Medullary Carcinoma"] and sf.grouped_recurrence_score IN ["16-20"]and d.tumor_size_group In ["(2,3]"] and tp.chemotherapy_regimen In ["FEC (3 week cycles)"]
-RETURN  f.file_name AS `File Name`,
-    head(labels(samp)) AS `Association`,
-    f.file_description AS `Description`,
-    f.file_format AS `File Format`,
-    f.file_size AS `Size`,
-    p.program_acronym AS `Program Code`,
-    s.study_acronym AS `Arm`,
-    ss.study_subject_id AS `Case ID`,
-    samp.sample_id AS `Sample ID`,
-    ss.disease_subtype as `Diagnosis`</t>
-  </si>
-  <si>
     <t>MATCH (ss:study_subject)
+MATCH (ss)&lt;-[:sample_of_study_subject]-(sp)&lt;-[:file_of_sample]-(f)-[:file_of_laboratory_procedure]-&gt;(lp)
+WITH ss, collect(DISTINCT sp.sample_id) AS samples, collect(DISTINCT lp.laboratory_procedure_id) AS lab_procedures, collect(DISTINCT f) AS files
+MATCH (ss)-[:study_subject_of_study]-&gt;(s)-[:study_of_program]-&gt;(p)
 MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
 MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
 MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
-WHERE ss.disease_subtype IN ["Medullary Carcinoma"] and sf.grouped_recurrence_score IN ["16-20"]and d.tumor_size_group In ["(2,3]"] and tp.chemotherapy_regimen In ["FEC (3 week cycles)"]
-WITH ss
-MATCH (ss)-[:study_subject_of_study]-&gt;(s)
-MATCH (s)-[:study_of_program]-&gt;(p)
-MATCH (ss)&lt;-[:sample_of_study_subject]-(samp)
-MATCH (samp)&lt;-[:file_of_sample]-(f)
-MATCH (lp)&lt;-[:file_of_laboratory_procedure]-(f)
-RETURN COUNT(DISTINCT p) AS Programs,
-COUNT(DISTINCT s) AS Arms,
-COUNT(DISTINCT ss) AS Cases,
-COUNT(DISTINCT samp) AS Samples,
-COUNT(DISTINCT lp) AS Assays,
-COUNT(DISTINCT f) AS Files</t>
+MATCH (ss)&lt;-[:demographic_of_study_subject]-(demo)
+WHERE ss.disease_subtype IN ["Medullary Carcinoma"] and sf.grouped_recurrence_score IN ["16-20"]and d.tumor_size_group In ["(2,3]"] and tp.chemotherapy_regimen In ["Other treatment given as part of a CTSU protocol"]
+return ss.study_subject_id as `Case ID`,
+       p.program_acronym as `Program Code`,
+        p.program_id as Program_ID,
+       s.study_acronym as `Arm`,
+       ss.disease_subtype as `Diagnosis`,
+       sf.grouped_recurrence_score AS `Recurrence Score`,
+       d.tumor_size_group AS `tumor_size`,
+       d.er_status AS `ER Status`,
+       d.pr_status AS `PR Status`,
+       demo.age_at_index AS `Age (years)`,
+demo.survival_time AS `Survival (days)`</t>
   </si>
 </sst>
 </file>
@@ -522,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -557,10 +557,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -574,10 +574,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -591,10 +591,10 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
updated bento scripts as per availability of objects for new data set
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Bento_MultiFilter_Diagnosis-Recurrence-TumorSize-Chemo_1.xlsx
+++ b/InputFiles/TC01_Bento_MultiFilter_Diagnosis-Recurrence-TumorSize-Chemo_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3D89D3-8382-4D9A-A92F-6EF760CD3BC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB319E90-AB1D-4303-9369-560A6651F8DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -63,11 +63,32 @@
     <t>TC01_Bento_MultiFilter_Diagnosis-Recurrence-TumorSize-Chemo_1_WebData.xlsx</t>
   </si>
   <si>
+    <t>MATCH (f:file)
+MATCH (f)-[:file_of_sample]-&gt;(samp)
+MATCH (samp)-[:sample_of_study_subject]-&gt;(ss)
+MATCH (ss)-[:study_subject_of_study]-&gt;(s)
+MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
+MATCH (s)-[:study_of_program]-&gt;(p)
+MATCH (d)-[:diagnosis_of_study_subject]-&gt;(ss)
+MATCH (tp)-[:tp_of_diagnosis]-&gt;(d)
+WHERE ss.disease_subtype IN ["Medullary Carcinoma"] and sf.grouped_recurrence_score IN ["31-35"]and d.tumor_size_group In ["(2,3]"] and tp.chemotherapy_regimen In ["Other treatment given as part of a CTSU protocol"]
+RETURN  f.file_name AS `File Name`,
+    head(labels(samp)) AS `Association`,
+    f.file_description AS `Description`,
+    f.file_format AS `File Format`,
+    f.file_size AS `Size`,
+    p.program_acronym AS `Program Code`,
+    s.study_acronym AS `Arm`,
+    ss.study_subject_id AS `Case ID`,
+    samp.sample_id AS `Sample ID`,
+    ss.disease_subtype as `Diagnosis`</t>
+  </si>
+  <si>
     <t>MATCH (ss:study_subject)
 MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
 MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
 MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
-WHERE ss.disease_subtype IN ["Medullary Carcinoma"] and sf.grouped_recurrence_score IN ["16-20"]and d.tumor_size_group In ["(2,3]"] and tp.chemotherapy_regimen In ["Other treatment given as part of a CTSU protocol"]
+WHERE ss.disease_subtype IN ["Medullary Carcinoma"] and sf.grouped_recurrence_score IN ["31-35"]and d.tumor_size_group In ["(2,3]"] and tp.chemotherapy_regimen In ["Other treatment given as part of a CTSU protocol"]
 WITH ss
 MATCH (ss)-[:study_subject_of_study]-&gt;(s)
 MATCH (s)-[:study_of_program]-&gt;(p)
@@ -82,25 +103,26 @@
 COUNT(DISTINCT f) AS Files</t>
   </si>
   <si>
-    <t>MATCH (f:file)
-MATCH (f)-[:file_of_sample]-&gt;(samp)
-MATCH (samp)-[:sample_of_study_subject]-&gt;(ss)
-MATCH (ss)-[:study_subject_of_study]-&gt;(s)
+    <t>MATCH (ss:study_subject)
+MATCH (ss)&lt;-[:sample_of_study_subject]-(sp)&lt;-[:file_of_sample]-(f)-[:file_of_laboratory_procedure]-&gt;(lp)
+WITH ss, collect(DISTINCT sp.sample_id) AS samples, collect(DISTINCT lp.laboratory_procedure_id) AS lab_procedures, collect(DISTINCT f) AS files
+MATCH (ss)-[:study_subject_of_study]-&gt;(s)-[:study_of_program]-&gt;(p)
 MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
-MATCH (s)-[:study_of_program]-&gt;(p)
-MATCH (d)-[:diagnosis_of_study_subject]-&gt;(ss)
-MATCH (tp)-[:tp_of_diagnosis]-&gt;(d)
-WHERE ss.disease_subtype IN ["Medullary Carcinoma"] and sf.grouped_recurrence_score IN ["16-20"]and d.tumor_size_group In ["(2,3]"] and tp.chemotherapy_regimen In ["Other treatment given as part of a CTSU protocol"]
-RETURN  f.file_name AS `File Name`,
-    head(labels(samp)) AS `Association`,
-    f.file_description AS `Description`,
-    f.file_format AS `File Format`,
-    f.file_size AS `Size`,
-    p.program_acronym AS `Program Code`,
-    s.study_acronym AS `Arm`,
-    ss.study_subject_id AS `Case ID`,
-    samp.sample_id AS `Sample ID`,
-    ss.disease_subtype as `Diagnosis`</t>
+MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
+MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
+MATCH (ss)&lt;-[:demographic_of_study_subject]-(demo)
+WHERE ss.disease_subtype IN ["Medullary Carcinoma"] and sf.grouped_recurrence_score IN ["31-35"]and d.tumor_size_group In ["(2,3]"] and tp.chemotherapy_regimen In ["Other treatment given as part of a CTSU protocol"]
+return ss.study_subject_id as `Case ID`,
+       p.program_acronym as `Program Code`,
+        p.program_id as Program_ID,
+       s.study_acronym as `Arm`,
+       ss.disease_subtype as `Diagnosis`,
+       sf.grouped_recurrence_score AS `Recurrence Score`,
+       d.tumor_size_group AS `tumor_size`,
+       d.er_status AS `ER Status`,
+       d.pr_status AS `PR Status`,
+       demo.age_at_index AS `Age (years)`,
+demo.survival_time AS `Survival (days)`</t>
   </si>
   <si>
     <t>MATCH (ss:study_subject)
@@ -112,7 +134,7 @@
 MATCH (samp)&lt;-[:file_of_sample]-(f)-[:file_of_laboratory_procedure]-&gt;(lp)
 MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
 MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
-WHERE ss.disease_subtype IN ["Medullary Carcinoma"] and sf.grouped_recurrence_score IN ["16-20"]and d.tumor_size_group In ["(2,3]"] and tp.chemotherapy_regimen In ["Other treatment given as part of a CTSU protocol"]
+WHERE ss.disease_subtype IN ["Medullary Carcinoma"] and sf.grouped_recurrence_score IN ["31-35"]and d.tumor_size_group In ["(2,3]"] and tp.chemotherapy_regimen In ["Other treatment given as part of a CTSU protocol"]
 WITH
     distinct lp,
     toInteger(split(ss.study_subject_id,'-')[2]) AS subject_id_num,
@@ -129,28 +151,6 @@
             samp.sample_anatomic_site AS `Sample Anatomic Site`,
             samp.method_of_sample_procurement AS `Sample Procurement Method`,
             lp.test_name as Platform</t>
-  </si>
-  <si>
-    <t>MATCH (ss:study_subject)
-MATCH (ss)&lt;-[:sample_of_study_subject]-(sp)&lt;-[:file_of_sample]-(f)-[:file_of_laboratory_procedure]-&gt;(lp)
-WITH ss, collect(DISTINCT sp.sample_id) AS samples, collect(DISTINCT lp.laboratory_procedure_id) AS lab_procedures, collect(DISTINCT f) AS files
-MATCH (ss)-[:study_subject_of_study]-&gt;(s)-[:study_of_program]-&gt;(p)
-MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
-MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
-MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
-MATCH (ss)&lt;-[:demographic_of_study_subject]-(demo)
-WHERE ss.disease_subtype IN ["Medullary Carcinoma"] and sf.grouped_recurrence_score IN ["16-20"]and d.tumor_size_group In ["(2,3]"] and tp.chemotherapy_regimen In ["Other treatment given as part of a CTSU protocol"]
-return ss.study_subject_id as `Case ID`,
-       p.program_acronym as `Program Code`,
-        p.program_id as Program_ID,
-       s.study_acronym as `Arm`,
-       ss.disease_subtype as `Diagnosis`,
-       sf.grouped_recurrence_score AS `Recurrence Score`,
-       d.tumor_size_group AS `tumor_size`,
-       d.er_status AS `ER Status`,
-       d.pr_status AS `PR Status`,
-       demo.age_at_index AS `Age (years)`,
-demo.survival_time AS `Survival (days)`</t>
   </si>
 </sst>
 </file>
@@ -522,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -557,10 +557,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -574,10 +574,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -591,10 +591,10 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
updated 4 scripts for bento perf
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Bento_MultiFilter_Diagnosis-Recurrence-TumorSize-Chemo_1.xlsx
+++ b/InputFiles/TC01_Bento_MultiFilter_Diagnosis-Recurrence-TumorSize-Chemo_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB319E90-AB1D-4303-9369-560A6651F8DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2236FB94-0BD0-4417-90BE-88DFE920F48D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -63,32 +63,33 @@
     <t>TC01_Bento_MultiFilter_Diagnosis-Recurrence-TumorSize-Chemo_1_WebData.xlsx</t>
   </si>
   <si>
-    <t>MATCH (f:file)
-MATCH (f)-[:file_of_sample]-&gt;(samp)
-MATCH (samp)-[:sample_of_study_subject]-&gt;(ss)
-MATCH (ss)-[:study_subject_of_study]-&gt;(s)
+    <t>MATCH (ss:study_subject)
+MATCH (ss)&lt;-[:sample_of_study_subject]-(sp)&lt;-[:file_of_sample]-(f)-[:file_of_laboratory_procedure]-&gt;(lp)
+WITH ss, collect(DISTINCT sp.sample_id) AS samples, collect(DISTINCT lp.laboratory_procedure_id) AS lab_procedures, collect(DISTINCT f) AS files
+MATCH (ss)-[:study_subject_of_study]-&gt;(s)-[:study_of_program]-&gt;(p)
 MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
-MATCH (s)-[:study_of_program]-&gt;(p)
-MATCH (d)-[:diagnosis_of_study_subject]-&gt;(ss)
-MATCH (tp)-[:tp_of_diagnosis]-&gt;(d)
-WHERE ss.disease_subtype IN ["Medullary Carcinoma"] and sf.grouped_recurrence_score IN ["31-35"]and d.tumor_size_group In ["(2,3]"] and tp.chemotherapy_regimen In ["Other treatment given as part of a CTSU protocol"]
-RETURN  f.file_name AS `File Name`,
-    head(labels(samp)) AS `Association`,
-    f.file_description AS `Description`,
-    f.file_format AS `File Format`,
-    f.file_size AS `Size`,
-    p.program_acronym AS `Program Code`,
-    s.study_acronym AS `Arm`,
-    ss.study_subject_id AS `Case ID`,
-    samp.sample_id AS `Sample ID`,
-    ss.disease_subtype as `Diagnosis`</t>
+MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
+MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
+MATCH (ss)&lt;-[:demographic_of_study_subject]-(demo)
+WHERE ss.disease_subtype IN ["Medullary Carcinoma"] and sf.grouped_recurrence_score IN ["16-20"]and d.tumor_size_group In ["(2,3]"] and tp.chemotherapy_regimen In ["Other treatment given as part of a CTSU protocol"]
+return ss.study_subject_id as `Case ID`,
+       p.program_acronym as `Program Code`,
+        p.program_id as Program_ID,
+       s.study_acronym as `Arm`,
+       ss.disease_subtype as `Diagnosis`,
+       sf.grouped_recurrence_score AS `Recurrence Score`,
+       d.tumor_size_group AS `tumor_size`,
+       d.er_status AS `ER Status`,
+       d.pr_status AS `PR Status`,
+       demo.age_at_index AS `Age (years)`,
+demo.survival_time AS `Survival (days)`</t>
   </si>
   <si>
     <t>MATCH (ss:study_subject)
 MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
 MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
 MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
-WHERE ss.disease_subtype IN ["Medullary Carcinoma"] and sf.grouped_recurrence_score IN ["31-35"]and d.tumor_size_group In ["(2,3]"] and tp.chemotherapy_regimen In ["Other treatment given as part of a CTSU protocol"]
+WHERE ss.disease_subtype IN ["Medullary Carcinoma"] and sf.grouped_recurrence_score IN ["16-20"] and d.tumor_size_group In ["(2,3]"] and tp.chemotherapy_regimen In ["Other treatment given as part of a CTSU protocol"]
 WITH ss
 MATCH (ss)-[:study_subject_of_study]-&gt;(s)
 MATCH (s)-[:study_of_program]-&gt;(p)
@@ -104,28 +105,6 @@
   </si>
   <si>
     <t>MATCH (ss:study_subject)
-MATCH (ss)&lt;-[:sample_of_study_subject]-(sp)&lt;-[:file_of_sample]-(f)-[:file_of_laboratory_procedure]-&gt;(lp)
-WITH ss, collect(DISTINCT sp.sample_id) AS samples, collect(DISTINCT lp.laboratory_procedure_id) AS lab_procedures, collect(DISTINCT f) AS files
-MATCH (ss)-[:study_subject_of_study]-&gt;(s)-[:study_of_program]-&gt;(p)
-MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
-MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
-MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
-MATCH (ss)&lt;-[:demographic_of_study_subject]-(demo)
-WHERE ss.disease_subtype IN ["Medullary Carcinoma"] and sf.grouped_recurrence_score IN ["31-35"]and d.tumor_size_group In ["(2,3]"] and tp.chemotherapy_regimen In ["Other treatment given as part of a CTSU protocol"]
-return ss.study_subject_id as `Case ID`,
-       p.program_acronym as `Program Code`,
-        p.program_id as Program_ID,
-       s.study_acronym as `Arm`,
-       ss.disease_subtype as `Diagnosis`,
-       sf.grouped_recurrence_score AS `Recurrence Score`,
-       d.tumor_size_group AS `tumor_size`,
-       d.er_status AS `ER Status`,
-       d.pr_status AS `PR Status`,
-       demo.age_at_index AS `Age (years)`,
-demo.survival_time AS `Survival (days)`</t>
-  </si>
-  <si>
-    <t>MATCH (ss:study_subject)
 WITH COLLECT(ss.study_subject_id) AS all_subjects
 MATCH (samp:sample)
 MATCH (samp)-[:sample_of_study_subject]-&gt;(ss)
@@ -134,7 +113,7 @@
 MATCH (samp)&lt;-[:file_of_sample]-(f)-[:file_of_laboratory_procedure]-&gt;(lp)
 MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
 MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
-WHERE ss.disease_subtype IN ["Medullary Carcinoma"] and sf.grouped_recurrence_score IN ["31-35"]and d.tumor_size_group In ["(2,3]"] and tp.chemotherapy_regimen In ["Other treatment given as part of a CTSU protocol"]
+WHERE ss.disease_subtype IN ["Medullary Carcinoma"] and sf.grouped_recurrence_score IN ["16-20"] and d.tumor_size_group In ["(2,3]"] and tp.chemotherapy_regimen In ["Other treatment given as part of a CTSU protocol"]
 WITH
     distinct lp,
     toInteger(split(ss.study_subject_id,'-')[2]) AS subject_id_num,
@@ -151,6 +130,27 @@
             samp.sample_anatomic_site AS `Sample Anatomic Site`,
             samp.method_of_sample_procurement AS `Sample Procurement Method`,
             lp.test_name as Platform</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)
+MATCH (f)-[:file_of_sample]-&gt;(samp)
+MATCH (samp)-[:sample_of_study_subject]-&gt;(ss)
+MATCH (ss)-[:study_subject_of_study]-&gt;(s)
+MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
+MATCH (s)-[:study_of_program]-&gt;(p)
+MATCH (d)-[:diagnosis_of_study_subject]-&gt;(ss)
+MATCH (tp)-[:tp_of_diagnosis]-&gt;(d)
+WHERE ss.disease_subtype IN ["Medullary Carcinoma"] and sf.grouped_recurrence_score IN ["16-20"] and d.tumor_size_group In ["(2,3]"] and tp.chemotherapy_regimen In ["Other treatment given as part of a CTSU protocol"]
+RETURN  f.file_name AS `File Name`,
+    head(labels(samp)) AS `Association`,
+    f.file_description AS `Description`,
+    f.file_format AS `File Format`,
+    f.file_size AS `Size`,
+    p.program_acronym AS `Program Code`,
+    s.study_acronym AS `Arm`,
+    ss.study_subject_id AS `Case ID`,
+    samp.sample_id AS `Sample ID`,
+    ss.disease_subtype as `Diagnosis`</t>
   </si>
 </sst>
 </file>
@@ -522,20 +522,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="75.81640625" customWidth="1"/>
-    <col min="3" max="3" width="60.453125" customWidth="1"/>
-    <col min="4" max="4" width="70.26953125" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.85546875" customWidth="1"/>
+    <col min="3" max="3" width="60.42578125" customWidth="1"/>
+    <col min="4" max="4" width="70.28515625" customWidth="1"/>
     <col min="5" max="5" width="53" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -552,12 +552,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="348" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="360" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>11</v>
@@ -569,12 +569,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="406" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>11</v>
@@ -586,12 +586,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="304.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="315" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>

</xml_diff>